<commit_message>
Add simple Buttons for GUI
</commit_message>
<xml_diff>
--- a/Applications/NewestFormNumber.xlsx
+++ b/Applications/NewestFormNumber.xlsx
@@ -1344,16 +1344,16 @@
     <row r="3" ht="20.25" customHeight="1" s="12">
       <c r="A3" s="5" t="n"/>
       <c r="B3" s="6" t="n">
-        <v>1012</v>
+        <v>1024</v>
       </c>
       <c r="C3" s="8" t="n">
-        <v>2001</v>
+        <v>2002</v>
       </c>
       <c r="D3" s="8" t="n">
-        <v>3001</v>
+        <v>3002</v>
       </c>
       <c r="E3" s="8" t="n">
-        <v>4001</v>
+        <v>4002</v>
       </c>
       <c r="F3" s="8" t="n"/>
       <c r="G3" s="8" t="n"/>

</xml_diff>

<commit_message>
implemented login + verfication + createForm
</commit_message>
<xml_diff>
--- a/Applications/NewestFormNumber.xlsx
+++ b/Applications/NewestFormNumber.xlsx
@@ -1,12 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet 1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
 </workbook>
@@ -1344,16 +1344,16 @@
     <row r="3" ht="20.25" customHeight="1" s="12">
       <c r="A3" s="5" t="n"/>
       <c r="B3" s="6" t="n">
-        <v>1025</v>
+        <v>1030</v>
       </c>
       <c r="C3" s="8" t="n">
-        <v>2002</v>
+        <v>2003</v>
       </c>
       <c r="D3" s="8" t="n">
-        <v>3002</v>
+        <v>3003</v>
       </c>
       <c r="E3" s="8" t="n">
-        <v>4002</v>
+        <v>4003</v>
       </c>
       <c r="F3" s="8" t="n"/>
       <c r="G3" s="8" t="n"/>

</xml_diff>